<commit_message>
yashwantraut: task h and v lookup
</commit_message>
<xml_diff>
--- a/Task H and V looup.xlsx
+++ b/Task H and V looup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data Analytics\Excel\task 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E277D9-B00A-45FD-AA26-456959B41EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCCD040-4F98-48FC-A285-232643E38AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{0DA197BB-6701-46E9-BA25-BD5B18E4213F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Emp ID</t>
   </si>
@@ -109,79 +109,46 @@
     <t>Kolkata</t>
   </si>
   <si>
-    <t>Product ID</t>
-  </si>
-  <si>
-    <t>P001</t>
-  </si>
-  <si>
-    <t>P002</t>
-  </si>
-  <si>
-    <t>P003</t>
-  </si>
-  <si>
-    <t>P004</t>
-  </si>
-  <si>
-    <t>P005</t>
-  </si>
-  <si>
-    <t>P006</t>
-  </si>
-  <si>
-    <t>P007</t>
-  </si>
-  <si>
-    <t>P008</t>
-  </si>
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Headphone</t>
-  </si>
-  <si>
-    <t>Keyboard</t>
-  </si>
-  <si>
-    <t>Washing Machine</t>
-  </si>
-  <si>
-    <t>Refrigerator</t>
-  </si>
-  <si>
-    <t>Chair</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>Accessories</t>
-  </si>
-  <si>
-    <t>Home Appliance</t>
-  </si>
-  <si>
-    <t>Furniture</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Stock</t>
+    <t>City code</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City Name </t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>karnataka</t>
+  </si>
+  <si>
+    <t>Tamil nadu</t>
+  </si>
+  <si>
+    <t>west Bengal</t>
+  </si>
+  <si>
+    <t>Population</t>
   </si>
 </sst>
 </file>
@@ -226,13 +193,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -275,12 +242,10 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,165 +797,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB1D64D-14A4-4018-8E35-EC07FF7268D9}">
-  <dimension ref="D5:L9"/>
+  <dimension ref="C6:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:L9"/>
+      <selection activeCell="D7" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="11.21875" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D5" s="4" t="s">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="D7" s="5" t="str">
+        <f>HLOOKUP(D6,$C$15:$F$17,2,FALSE)</f>
+        <v>Mumbai</v>
+      </c>
+      <c r="E7" s="5" t="str">
+        <f t="shared" ref="E7:F7" si="0">HLOOKUP(E6,$C$15:$F$17,2,FALSE)</f>
+        <v>Maharashtra</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6">
+        <v>19000000</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="D9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="6">
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="D10" s="5" t="str">
+        <f>HLOOKUP(D6,$C$15:$F$17,3,FALSE)</f>
+        <v>Chennai</v>
+      </c>
+      <c r="E10" s="5" t="str">
+        <f t="shared" ref="E10:F10" si="1">HLOOKUP(E6,$C$15:$F$17,3,FALSE)</f>
+        <v>Tamil nadu</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="1"/>
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="D11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="6">
+        <v>11000000</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="4:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D6" s="5" t="s">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="7">
+        <v>2000000</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="5" t="s">
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="6">
+        <v>9000000</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="4:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="5">
-        <v>50000</v>
-      </c>
-      <c r="F8" s="5">
-        <v>25000</v>
-      </c>
-      <c r="G8" s="5">
-        <v>2000</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1200</v>
-      </c>
-      <c r="I8" s="5">
-        <v>30000</v>
-      </c>
-      <c r="J8" s="5">
-        <v>40000</v>
-      </c>
-      <c r="K8" s="5">
-        <v>5000</v>
-      </c>
-      <c r="L8" s="5">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="5">
-        <v>20</v>
-      </c>
-      <c r="F9" s="5">
-        <v>35</v>
-      </c>
-      <c r="G9" s="5">
-        <v>50</v>
-      </c>
-      <c r="H9" s="5">
-        <v>40</v>
-      </c>
-      <c r="I9" s="5">
-        <v>15</v>
-      </c>
-      <c r="J9" s="5">
-        <v>10</v>
-      </c>
-      <c r="K9" s="5">
-        <v>25</v>
-      </c>
-      <c r="L9" s="5">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yashwantraut: craete task h and v lookup
</commit_message>
<xml_diff>
--- a/Task H and V looup.xlsx
+++ b/Task H and V looup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data Analytics\Excel\task 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCCD040-4F98-48FC-A285-232643E38AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FF6F25-254E-43C5-9B3E-6F1F6032A3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{0DA197BB-6701-46E9-BA25-BD5B18E4213F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Emp ID</t>
   </si>
@@ -231,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -245,7 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,10 +796,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB1D64D-14A4-4018-8E35-EC07FF7268D9}">
-  <dimension ref="C6:F17"/>
+  <dimension ref="C6:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F7"/>
+      <selection activeCell="D11" sqref="D11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,7 +831,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="5" t="str">
-        <f>HLOOKUP(D6,$C$15:$F$17,2,FALSE)</f>
+        <f>HLOOKUP(D6,$C15:$F17,2,FALSE)</f>
         <v>Mumbai</v>
       </c>
       <c r="E7" s="5" t="str">
@@ -848,13 +847,16 @@
       <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="D8" s="5" t="str">
+        <f>HLOOKUP(D6,$C$15:$F$20,4,FALSE)</f>
+        <v>Delhi</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <f t="shared" ref="E8:F8" si="1">HLOOKUP(E6,$C$15:$F$20,4,FALSE)</f>
+        <v>Delhi</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="1"/>
         <v>19000000</v>
       </c>
     </row>
@@ -862,13 +864,16 @@
       <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="D9" s="5" t="str">
+        <f>HLOOKUP(D6,$C15:$F20,5,FALSE)</f>
+        <v>karnataka</v>
+      </c>
+      <c r="E9" s="5" t="str">
+        <f t="shared" ref="E9:F9" si="2">HLOOKUP(E6,$C15:$F20,5,FALSE)</f>
+        <v>Bengaluru</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="2"/>
         <v>12000000</v>
       </c>
     </row>
@@ -881,11 +886,11 @@
         <v>Chennai</v>
       </c>
       <c r="E10" s="5" t="str">
-        <f t="shared" ref="E10:F10" si="1">HLOOKUP(E6,$C$15:$F$17,3,FALSE)</f>
+        <f t="shared" ref="E10:F10" si="3">HLOOKUP(E6,$C$15:$F$17,3,FALSE)</f>
         <v>Tamil nadu</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9000000</v>
       </c>
     </row>
@@ -893,13 +898,16 @@
       <c r="C11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="D11" s="5" t="str">
+        <f>HLOOKUP(D6,$C15:F420,6,FALSE)</f>
+        <v>Kolkata</v>
+      </c>
+      <c r="E11" s="5" t="str">
+        <f>HLOOKUP(E6,$C15:G420,6,FALSE)</f>
+        <v>west Bengal</v>
+      </c>
+      <c r="F11" s="5">
+        <f>HLOOKUP(F6,$C15:H420,6,FALSE)</f>
         <v>11000000</v>
       </c>
     </row>
@@ -921,7 +929,7 @@
       <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <v>2000000</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -943,6 +951,48 @@
       </c>
       <c r="F17" s="5" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="6">
+        <v>19000000</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="6">
+        <v>12000000</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="6">
+        <v>11000000</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>